<commit_message>
covered maths and comparison operator, and cell referencing
</commit_message>
<xml_diff>
--- a/0_Resources/Problems/2_Formulas_Functions/1_Formulas_Intro.xlsx
+++ b/0_Resources/Problems/2_Formulas_Functions/1_Formulas_Intro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Okoko\Desktop\DATA ANALYSIS PROJECT\EXCEL PROJECTS\excel_data_analytics_project\0_Resources\Problems\2_Formulas_Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EC0EF2-CEB1-417F-AC06-B23DB21E77EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CEB35F-2DE4-4A34-A1E8-D7BB169B20CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8CC555B5-3E06-43B6-9E5B-C0A1D3498DA4}"/>
   </bookViews>
@@ -414,7 +414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -487,6 +487,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A41B6C-80F1-4D7E-AD46-00EDEBFEC87C}">
   <dimension ref="B1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +840,9 @@
     <col min="4" max="4" width="12.28515625" style="4" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="4" customWidth="1"/>
     <col min="6" max="6" width="10" style="4" customWidth="1"/>
-    <col min="7" max="13" width="9" style="4"/>
+    <col min="7" max="7" width="9" style="4"/>
+    <col min="8" max="8" width="9" style="30"/>
+    <col min="9" max="13" width="9" style="4"/>
     <col min="14" max="14" width="11.28515625" style="4" customWidth="1"/>
     <col min="15" max="16384" width="9" style="4"/>
   </cols>
@@ -861,7 +867,7 @@
       <c r="G2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="31" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="23" t="s">
@@ -907,9 +913,37 @@
         <f>D3+E3</f>
         <v>130000</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="30">
         <f>E3/D3</f>
         <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I3" s="4">
+        <f>H3 * D3</f>
+        <v>10000</v>
+      </c>
+      <c r="J3" s="4" t="b">
+        <f>I3=E3</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="4" t="b">
+        <f>E3&gt;D3</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="4" t="b">
+        <f>C3&lt;=$C$15</f>
+        <v>1</v>
+      </c>
+      <c r="M3" s="4" t="b">
+        <f>D3&gt;=$C$16</f>
+        <v>1</v>
+      </c>
+      <c r="N3" s="4">
+        <f>L3 *M3</f>
+        <v>1</v>
+      </c>
+      <c r="O3" s="4" t="b">
+        <f>N3=1</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
@@ -933,9 +967,37 @@
         <f t="shared" ref="G4:G12" si="1">D4+E4</f>
         <v>147000</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="30">
         <f t="shared" ref="H4:H12" si="2">E4/D4</f>
         <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" ref="I4:I12" si="3">H4 * D4</f>
+        <v>12000</v>
+      </c>
+      <c r="J4" s="4" t="b">
+        <f t="shared" ref="J4:J12" si="4">I4=E4</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="4" t="b">
+        <f t="shared" ref="K4:K12" si="5">E4&gt;D4</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="4" t="b">
+        <f t="shared" ref="L4:L12" si="6">C4&lt;=$C$15</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="4" t="b">
+        <f t="shared" ref="M4:M12" si="7">D4&gt;=$C$16</f>
+        <v>1</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" ref="N4:N12" si="8">L4 *M4</f>
+        <v>1</v>
+      </c>
+      <c r="O4" s="4" t="b">
+        <f t="shared" ref="O4:O12" si="9">N4=1</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
@@ -959,9 +1021,37 @@
         <f t="shared" si="1"/>
         <v>80000</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="30">
         <f t="shared" si="2"/>
         <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="J5" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M5" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
@@ -985,9 +1075,37 @@
         <f t="shared" si="1"/>
         <v>118000</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="30">
         <f t="shared" si="2"/>
         <v>7.2727272727272724E-2</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="3"/>
+        <v>8000</v>
+      </c>
+      <c r="J6" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -1011,9 +1129,37 @@
         <f t="shared" si="1"/>
         <v>136000</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="30">
         <f t="shared" si="2"/>
         <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="3"/>
+        <v>11000</v>
+      </c>
+      <c r="J7" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K7" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M7" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O7" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
@@ -1037,9 +1183,37 @@
         <f t="shared" si="1"/>
         <v>97000</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="30">
         <f t="shared" si="2"/>
         <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="3"/>
+        <v>7000</v>
+      </c>
+      <c r="J8" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -1063,9 +1237,37 @@
         <f t="shared" si="1"/>
         <v>165000</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="30">
         <f t="shared" si="2"/>
         <v>0.1</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="3"/>
+        <v>15000</v>
+      </c>
+      <c r="J9" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -1089,9 +1291,37 @@
         <f t="shared" si="1"/>
         <v>143000</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="30">
         <f t="shared" si="2"/>
         <v>0.1</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="3"/>
+        <v>13000</v>
+      </c>
+      <c r="J10" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K10" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -1115,9 +1345,37 @@
         <f t="shared" si="1"/>
         <v>154000</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="30">
         <f t="shared" si="2"/>
         <v>0.1</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="3"/>
+        <v>14000</v>
+      </c>
+      <c r="J11" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K11" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M11" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O11" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1141,9 +1399,37 @@
         <f t="shared" si="1"/>
         <v>124000</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="30">
         <f t="shared" si="2"/>
         <v>7.8260869565217397E-2</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="3"/>
+        <v>9000</v>
+      </c>
+      <c r="J12" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K12" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M12" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O12" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1155,13 +1441,17 @@
       <c r="B15" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="26">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="28"/>
+      <c r="C16" s="28">
+        <v>80000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>